<commit_message>
test des regles et mapping
</commit_message>
<xml_diff>
--- a/scripts/CIUSS_TKFH_Serv.Pharmacy_2019_essai.xlsx
+++ b/scripts/CIUSS_TKFH_Serv.Pharmacy_2019_essai.xlsx
@@ -551,13 +551,16 @@
   <dimension ref="A1:M1201"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="J23"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="25.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -626,9 +629,7 @@
       <c r="H2" s="0" t="n">
         <v>56</v>
       </c>
-      <c r="I2" s="2" t="n">
-        <v>43466.3055208333</v>
-      </c>
+      <c r="I2" s="2"/>
       <c r="J2" s="2" t="n">
         <v>43466.4200347222</v>
       </c>

</xml_diff>